<commit_message>
aaded with ability to take ss without ISI and cookies alert
</commit_message>
<xml_diff>
--- a/urls.XLSX
+++ b/urls.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sandbox\javascript\screenshot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB1A6F4-6E85-4BCE-BE2B-507C205C5CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A0AB3-5D6E-42D8-9553-9A5B8F827ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,30 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.rybelsus.com/savings-and-support.html</t>
+  </si>
   <si>
     <t>https://www.rybelsus.com/</t>
-  </si>
-  <si>
-    <t>https://www.rybelsus.com/why-rybelsus/rybelsus-results.html</t>
-  </si>
-  <si>
-    <t>https://www.rybelsus.com/why-rybelsus/rybelsus-vs-other-diabetes-pills.html</t>
-  </si>
-  <si>
-    <t>https://www.rybelsus.com/why-rybelsus/how-rybelsus-works.html</t>
-  </si>
-  <si>
-    <t>https://www.rybelsus.com/why-rybelsus/real-rybelsus-stories.html</t>
-  </si>
-  <si>
-    <t>https://www.rybelsus.com/taking-rybelsus/how-to-start-rybelsus.html</t>
-  </si>
-  <si>
-    <t>https://www.rybelsus.com/taking-rybelsus/what-to-expect-with-rybelsus.html</t>
-  </si>
-  <si>
-    <t>URL</t>
   </si>
 </sst>
 </file>
@@ -373,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,12 +371,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -399,31 +384,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added fuction to calculate time for whole process
</commit_message>
<xml_diff>
--- a/urls.XLSX
+++ b/urls.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sandbox\javascript\screenshot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A0AB3-5D6E-42D8-9553-9A5B8F827ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C77A999-756D-4489-80D6-03CA46AC4057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>URL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>https://www.rybelsus.com/savings-and-support.html</t>
   </si>
   <si>
     <t>https://www.rybelsus.com/</t>
+  </si>
+  <si>
+    <t>EN_URL</t>
+  </si>
+  <si>
+    <t>ES_URL</t>
+  </si>
+  <si>
+    <t>https://espanol.rybelsus.com/</t>
+  </si>
+  <si>
+    <t>https://espanol.rybelsus.com/ahorros-y-apoyo.html</t>
   </si>
 </sst>
 </file>
@@ -49,6 +58,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Consolas"/>
@@ -358,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,19 +379,28 @@
     <col min="1" max="1" width="73.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added function to save ES SS as well
</commit_message>
<xml_diff>
--- a/urls.XLSX
+++ b/urls.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sandbox\javascript\screenshot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C77A999-756D-4489-80D6-03CA46AC4057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5AC1C8-D3E8-489A-A735-B5A485258525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>https://www.rybelsus.com/savings-and-support.html</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>https://www.rybelsus.com/</t>
   </si>
@@ -40,9 +37,6 @@
   </si>
   <si>
     <t>https://espanol.rybelsus.com/</t>
-  </si>
-  <si>
-    <t>https://espanol.rybelsus.com/ahorros-y-apoyo.html</t>
   </si>
 </sst>
 </file>
@@ -368,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,26 +375,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert back to En Es folder verion. with some code update
</commit_message>
<xml_diff>
--- a/urls.XLSX
+++ b/urls.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sandbox\javascript\screenshot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4495F6-C084-4EFD-9656-3078027D2D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BF8B2D-94FE-4B36-A7B7-FFC93A40856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>https://www.rybelsus.com/</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>https://espanol.rybelsus.com/</t>
-  </si>
-  <si>
-    <t>https://www.rybelsus.com/about-type-2-diabetes/type-2-diabetes-lifestyle-tips.html</t>
-  </si>
-  <si>
-    <t>https://espanol.rybelsus.com/ahorros-y-apoyo.html</t>
   </si>
 </sst>
 </file>
@@ -368,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -395,14 +389,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>